<commit_message>
Updated company list and pipeline visualization
- Added comprehensive README documentation with visual pipeline
- Enhanced web scraping with Google, DuckDuckGo, and Perplexity
- Updated to 17 companies with adjusted metric weights
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,63 +520,42 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LiveDesign (Schrödinger)</t>
+          <t>Revvity</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ReSync</t>
+          <t>Sapio</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Revvity</t>
+          <t>SciNote</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sapio</t>
+          <t>Scispot</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SciNote</t>
+          <t>SimulationsPlus</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Scispot</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SimulationsPlus</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
           <t>tetrascience</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Thermo Scientific</t>
         </is>
       </c>
     </row>

</xml_diff>